<commit_message>
update test 5 and test 6
</commit_message>
<xml_diff>
--- a/boltz_experiment_master.xlsx
+++ b/boltz_experiment_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39b8f5b1ceed89e2/Desktop/MSc_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{5F9DF5E2-6C68-4678-AFC6-E59FBBEA935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84E7311E-D115-4A76-9ADD-64F07E2760C8}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{5F9DF5E2-6C68-4678-AFC6-E59FBBEA935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFFEE9B2-E889-4DDB-AA34-3041EB121F5D}"/>
   <bookViews>
-    <workbookView xWindow="550" yWindow="0" windowWidth="15660" windowHeight="11280" xr2:uid="{B693CC76-476B-46BE-908F-567C50EF84D4}"/>
+    <workbookView xWindow="2880" yWindow="220" windowWidth="15660" windowHeight="11280" xr2:uid="{B693CC76-476B-46BE-908F-567C50EF84D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment tracking" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
   <si>
     <t>Experiment ID</t>
   </si>
@@ -218,6 +218,44 @@
   </si>
   <si>
     <t>The relative positions of the extracellular and intracellular domains remain stable after adding the eight ligands.</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>005_fgfr2_ligand_x50.yaml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>added 50 ligands</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>005_fgfr2_ligand_x50_model.cif</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Since the number of ligands is too large, the CIF file cannot be opened properly. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>006_fgfr2_ECD_ICD_torsion.yaml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Separate ECD and ICD via CXC file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>006_fgfr2_ECD_ICD_torsion.cif</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The two domains appear to be successfully separated, although the ECD still shows interactions with the TM region.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -647,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155A3948-C683-4751-821F-C1EF1E91D33B}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -841,6 +879,76 @@
       </c>
       <c r="K5" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test 7 and test 8 update
</commit_message>
<xml_diff>
--- a/boltz_experiment_master.xlsx
+++ b/boltz_experiment_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39b8f5b1ceed89e2/Desktop/MSc_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{5F9DF5E2-6C68-4678-AFC6-E59FBBEA935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFFEE9B2-E889-4DDB-AA34-3041EB121F5D}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{5F9DF5E2-6C68-4678-AFC6-E59FBBEA935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F261FCD-4EC3-4698-B7D0-2C9BD20FB552}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="220" windowWidth="15660" windowHeight="11280" xr2:uid="{B693CC76-476B-46BE-908F-567C50EF84D4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B693CC76-476B-46BE-908F-567C50EF84D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment tracking" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
   <si>
     <t>Experiment ID</t>
   </si>
@@ -255,6 +255,58 @@
   </si>
   <si>
     <t>The two domains appear to be successfully separated, although the ECD still shows interactions with the TM region.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platform</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google Colab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>007_fgfr2_ECD_ICD_constraints.yaml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>007_fgfr2_ECD_ICD_constraints.cif</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Since no minimum distance is defined in the constraint setup, I set the maximum distance to a very large value (100).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Constraints tend to enforce contact between the two domains rather than separate them.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008_fgfr2_ligand_x7.yaml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>added eight ligands</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008_fgfr2_ligand_x7_model.cif</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Since I could not reproduce Test 4 due to GPU limitations on Google Colab, I tested the maximum number of ligands I can add without using Colab Pro.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The maximum number of ligands we can include without a Google Colab Pro subscription is seven.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -685,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155A3948-C683-4751-821F-C1EF1E91D33B}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -700,13 +752,14 @@
     <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.36328125" customWidth="1"/>
     <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.08984375" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,10 +791,13 @@
         <v>39</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -773,10 +829,13 @@
         <v>24</v>
       </c>
       <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -808,10 +867,13 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -843,10 +905,13 @@
         <v>24</v>
       </c>
       <c r="K4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -869,7 +934,7 @@
         <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="I5" t="s">
         <v>48</v>
@@ -878,10 +943,13 @@
         <v>24</v>
       </c>
       <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -913,10 +981,13 @@
         <v>24</v>
       </c>
       <c r="K6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -927,13 +998,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
@@ -948,7 +1019,86 @@
         <v>24</v>
       </c>
       <c r="K7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>